<commit_message>
Added analysis year 2
</commit_message>
<xml_diff>
--- a/data/basketball_season1_prepost_codebook.xlsx
+++ b/data/basketball_season1_prepost_codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11106"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonkalen/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sok-anton/Documents/repos/basketball-coaching-teams/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A1B055-FCEB-AD48-B734-FCE56852E0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C7FDC1-B56E-DD4B-915B-809A624C361B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="29300" windowWidth="28800" windowHeight="17500" xr2:uid="{589E54C0-5F68-8340-878E-D726C5F7BFE7}"/>
+    <workbookView xWindow="1200" yWindow="500" windowWidth="27600" windowHeight="17500" xr2:uid="{589E54C0-5F68-8340-878E-D726C5F7BFE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="146">
   <si>
     <t>variable</t>
   </si>
@@ -413,9 +413,6 @@
     <t>Jag tycker att rollfördelningen i vår stab fungerar bra.</t>
   </si>
   <si>
-    <t>Jag tycker att samarbetet staben gör att vi presterar bättre än vad vi hade gjort om vi hade arbetat individuellt.</t>
-  </si>
-  <si>
     <t>Jag har hittat en roll som passar mig i min stab.</t>
   </si>
   <si>
@@ -429,6 +426,54 @@
   </si>
   <si>
     <t>Samarbetet i staben under match fungerar bra</t>
+  </si>
+  <si>
+    <t>year_2022</t>
+  </si>
+  <si>
+    <t>year_2023</t>
+  </si>
+  <si>
+    <t>participate_last_year</t>
+  </si>
+  <si>
+    <t>Var du med som coach i landslaget förra året?</t>
+  </si>
+  <si>
+    <t>Coach förra året</t>
+  </si>
+  <si>
+    <t>Hur många gånger har ni i er stab haft kontakt fram till dagens datum?</t>
+  </si>
+  <si>
+    <t>contact_pre</t>
+  </si>
+  <si>
+    <t>Antal kontakter innan säsong</t>
+  </si>
+  <si>
+    <t>contact_post</t>
+  </si>
+  <si>
+    <t>Antal kontakter under säsong</t>
+  </si>
+  <si>
+    <t>Jag tycker att samarbetet i staben gör att vi presterar bättre än vad vi hade gjort om vi hade arbetat individuellt.</t>
+  </si>
+  <si>
+    <t>Hur har din generella upplevelse att vara landslagscoach varit denna säsong?</t>
+  </si>
+  <si>
+    <t>general_experience</t>
+  </si>
+  <si>
+    <t>performance_game</t>
+  </si>
+  <si>
+    <t>performance_collaboration</t>
+  </si>
+  <si>
+    <t>Hur upplever du att sammarbetet i staben har påverkat lagets prestation som helhet?</t>
   </si>
 </sst>
 </file>
@@ -786,19 +831,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86AD8FB-9683-DC40-9C59-3C5C5474A18B}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="92.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="92.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -808,8 +853,14 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -819,8 +870,14 @@
       <c r="C2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -830,610 +887,1022 @@
       <c r="C3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
         <v>31</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" t="s">
         <v>32</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B18" t="s">
         <v>33</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>34</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>49</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>35</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
         <v>50</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C20" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
         <v>51</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C21" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" t="s">
         <v>52</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C22" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" t="s">
         <v>53</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C23" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>39</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" t="s">
         <v>54</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>40</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>55</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>41</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" t="s">
         <v>56</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C26" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>42</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" t="s">
         <v>57</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C27" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>43</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" t="s">
         <v>58</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C28" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>44</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" t="s">
         <v>59</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>45</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" t="s">
         <v>60</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C30" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>46</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" t="s">
         <v>61</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>47</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B32" t="s">
         <v>62</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C32" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>48</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B33" t="s">
         <v>63</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C33" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>69</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B34" t="s">
         <v>64</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C34" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>70</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B35" t="s">
         <v>115</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C35" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>71</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B36" t="s">
         <v>116</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C36" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>72</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" t="s">
         <v>67</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C37" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>73</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>68</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C38" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>74</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B39" t="s">
         <v>121</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C39" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>75</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B40" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" t="s">
+        <v>122</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" t="s">
         <v>125</v>
       </c>
-      <c r="C37" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>76</v>
-      </c>
-      <c r="B38" t="s">
-        <v>124</v>
-      </c>
-      <c r="C38" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>77</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="C42" t="s">
+        <v>125</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>144</v>
+      </c>
+      <c r="C45" t="s">
+        <v>145</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" t="s">
         <v>126</v>
       </c>
-      <c r="C39" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>78</v>
-      </c>
-      <c r="B40" t="s">
-        <v>117</v>
-      </c>
-      <c r="C40" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>78</v>
-      </c>
-      <c r="B41" t="s">
-        <v>118</v>
-      </c>
-      <c r="C41" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" t="s">
-        <v>79</v>
-      </c>
-      <c r="C42" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" t="s">
-        <v>83</v>
-      </c>
-      <c r="C44" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="C49" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" t="s">
         <v>127</v>
       </c>
-      <c r="C45" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>88</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="C50" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" t="s">
         <v>128</v>
       </c>
-      <c r="C46" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>90</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="C51" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" t="s">
         <v>129</v>
       </c>
-      <c r="C47" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>111</v>
-      </c>
-      <c r="B48" t="s">
-        <v>130</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="C52" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>91</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B53" t="s">
         <v>98</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C53" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>92</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B54" t="s">
         <v>99</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C54" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>93</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B55" t="s">
         <v>100</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C55" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>94</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B56" t="s">
         <v>101</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C56" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>95</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B57" t="s">
         <v>102</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C57" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>96</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B58" t="s">
         <v>103</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C58" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>97</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B59" t="s">
         <v>104</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C59" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>105</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B60" t="s">
         <v>106</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C60" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>107</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B61" t="s">
         <v>108</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C61" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>110</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B62" t="s">
         <v>109</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C62" t="s">
         <v>109</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>142</v>
+      </c>
+      <c r="C63" t="s">
+        <v>141</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>